<commit_message>
Diverse Updates, siehe Email
</commit_message>
<xml_diff>
--- a/ki2va_WirL_Matrix_20171208.xlsx
+++ b/ki2va_WirL_Matrix_20171208.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="23280" yWindow="440" windowWidth="28440" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7600" yWindow="8340" windowWidth="28440" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle2" sheetId="2" r:id="rId1"/>
@@ -792,10 +792,10 @@
   <dimension ref="A1:U26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="G15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I29" sqref="I29"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>